<commit_message>
board, add v1.0 single-board design
Includes buck converter for 26V operation. Component positions and
rotations validated against design/JLCPCB assembly preview.
</commit_message>
<xml_diff>
--- a/pcb/owl-driver-board-bom.xlsx
+++ b/pcb/owl-driver-board-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="109">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -47,6 +47,7 @@
         <color rgb="FFAFABAB"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -66,6 +67,7 @@
         <color rgb="FFAFABAB"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -83,7 +85,7 @@
     <t xml:space="preserve">0.1uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C6,C9,C11</t>
+    <t xml:space="preserve">C6,C9</t>
   </si>
   <si>
     <t xml:space="preserve">Capacitor_SMD:C_0603_1608Metric</t>
@@ -95,7 +97,7 @@
     <t xml:space="preserve">10uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C1,C2,C3,C4,C5,C7,C8,C10,C12</t>
+    <t xml:space="preserve">C1,C2,C3,C5,C12,C14</t>
   </si>
   <si>
     <t xml:space="preserve">Capacitor_SMD:C_1206_3216Metric</t>
@@ -104,7 +106,31 @@
     <t xml:space="preserve">C13585</t>
   </si>
   <si>
-    <t xml:space="preserve">SMBJ14A</t>
+    <t xml:space="preserve">100uF Tantalum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor_Tantalum_SMD:CP_EIA-3528-21_Kemet-B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C16133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220uF Electrolytic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radial_8x7mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C216322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMBJ26A</t>
   </si>
   <si>
     <t xml:space="preserve">D7</t>
@@ -113,7 +139,7 @@
     <t xml:space="preserve">Diode_SMD:D_SMB_Handsoldering</t>
   </si>
   <si>
-    <t xml:space="preserve">C315990</t>
+    <t xml:space="preserve">C315992</t>
   </si>
   <si>
     <t xml:space="preserve">SMBJ5.0A</t>
@@ -140,7 +166,7 @@
     <t xml:space="preserve">SZYY0805R</t>
   </si>
   <si>
-    <t xml:space="preserve">D1,D4,D5,D19,D20,D29</t>
+    <t xml:space="preserve">D1,D4,D5,D19,D20</t>
   </si>
   <si>
     <t xml:space="preserve">LED_SMD:LED_0805_2012Metric</t>
@@ -200,7 +226,7 @@
     <t xml:space="preserve">2920L200DR</t>
   </si>
   <si>
-    <t xml:space="preserve">F2,F3,F4,F5,F6</t>
+    <t xml:space="preserve">F2,F3,F4,F5</t>
   </si>
   <si>
     <t xml:space="preserve">C207087</t>
@@ -314,25 +340,37 @@
     <t xml:space="preserve">470R</t>
   </si>
   <si>
-    <t xml:space="preserve">R1,R4,R5,R6,R7,R9,R10,R15,R16,R17,R18,R19,R20,R23,R24,R25,R26,R27,R29,R30,R31,R38</t>
+    <t xml:space="preserve">R1,R4,R5,R6,R7,R9,R10,R15,R16,R17,R18,R19,R20,R24,R25,R26,R27,R29,R30,R31,R38</t>
   </si>
   <si>
     <t xml:space="preserve">C17710</t>
   </si>
   <si>
-    <t xml:space="preserve">AZ1117CH-5.0TRG1</t>
+    <t xml:space="preserve">Regulator-XL1509-SOIC8</t>
   </si>
   <si>
     <t xml:space="preserve">U1</t>
   </si>
   <si>
-    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6187</t>
+    <t xml:space="preserve">Package_SO:SOIC-8_3.9x4.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C61063</t>
   </si>
   <si>
     <t xml:space="preserve">SOT-223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68uH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inductor_SMD:L_10.4x10.4_H4.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C149549</t>
   </si>
   <si>
     <t xml:space="preserve">PCA9685PW</t>
@@ -401,6 +439,7 @@
       <color rgb="FFAFABAB"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <strike val="true"/>
@@ -459,7 +498,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -501,10 +540,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -585,10 +620,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -643,14 +678,14 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>0.0014</v>
       </c>
       <c r="H2" s="6" t="n">
         <f aca="false">G2*F2</f>
-        <v>0.0042</v>
+        <v>0.0028</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,14 +705,14 @@
         <v>14</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>0.0356</v>
       </c>
       <c r="H3" s="6" t="n">
         <f aca="false">G3*F3</f>
-        <v>0.3204</v>
+        <v>0.2492</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -697,14 +732,14 @@
         <v>18</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>0.3044</v>
+        <v>0.088</v>
       </c>
       <c r="H4" s="6" t="n">
         <f aca="false">G4*F4</f>
-        <v>0.3044</v>
+        <v>0.264</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -715,61 +750,61 @@
         <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>0.1477</v>
+        <v>0.062</v>
       </c>
       <c r="H5" s="6" t="n">
         <f aca="false">G5*F5</f>
-        <v>0.1477</v>
+        <v>0.062</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>0.0192</v>
+        <v>0.3044</v>
       </c>
       <c r="H6" s="6" t="n">
         <f aca="false">G6*F6</f>
-        <v>0.096</v>
+        <v>0.3044</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>29</v>
@@ -778,137 +813,131 @@
         <v>29</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>0.012</v>
+        <v>0.1477</v>
       </c>
       <c r="H7" s="6" t="n">
         <f aca="false">G7*F7</f>
-        <v>0.072</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>30</v>
+        <v>0.1477</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>0.0342</v>
+        <v>0.0192</v>
       </c>
       <c r="H8" s="6" t="n">
         <f aca="false">G8*F8</f>
-        <v>0.6156</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>35</v>
+        <v>0.096</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>0.0513</v>
+        <v>0.012</v>
       </c>
       <c r="H9" s="6" t="n">
         <f aca="false">G9*F9</f>
-        <v>0.2052</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>40</v>
+        <v>0.06</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>0.7053</v>
+        <v>0.0342</v>
       </c>
       <c r="H10" s="6" t="n">
         <f aca="false">G10*F10</f>
-        <v>0.7053</v>
+        <v>0.6156</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>0.3107</v>
+        <v>0.0513</v>
       </c>
       <c r="H11" s="6" t="n">
         <f aca="false">G11*F11</f>
-        <v>1.5535</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>45</v>
+        <v>0.2052</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -931,22 +960,25 @@
         <v>1</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.9372</v>
+        <v>0.7053</v>
       </c>
       <c r="H12" s="6" t="n">
         <f aca="false">G12*F12</f>
-        <v>0.9372</v>
+        <v>0.7053</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>56</v>
@@ -955,14 +987,17 @@
         <v>56</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.2165</v>
+        <v>0.3107</v>
       </c>
       <c r="H13" s="6" t="n">
         <f aca="false">G13*F13</f>
-        <v>1.0825</v>
+        <v>1.2428</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -972,58 +1007,58 @@
       <c r="B14" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.0221</v>
+        <v>0.9372</v>
       </c>
       <c r="H14" s="6" t="n">
         <f aca="false">G14*F14</f>
-        <v>0.0221</v>
+        <v>0.9372</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F15" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.043</v>
+        <v>0.2165</v>
       </c>
       <c r="H15" s="6" t="n">
         <f aca="false">G15*F15</f>
-        <v>0.043</v>
+        <v>1.0825</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1036,11 +1071,11 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>0.0116</v>
+        <v>0.0221</v>
       </c>
       <c r="H16" s="6" t="n">
         <f aca="false">G16*F16</f>
-        <v>0.0116</v>
+        <v>0.0221</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,51 +1085,51 @@
       <c r="B17" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="D17" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>0.0337</v>
+        <v>0.043</v>
       </c>
       <c r="H17" s="6" t="n">
         <f aca="false">G17*F17</f>
-        <v>0.0337</v>
+        <v>0.043</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F18" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>0.1947</v>
+        <v>0.0116</v>
       </c>
       <c r="H18" s="6" t="n">
         <f aca="false">G18*F18</f>
-        <v>0.9735</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>75</v>
+        <v>0.0116</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1104,9 +1139,6 @@
       <c r="B19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D19" s="1" t="s">
         <v>78</v>
       </c>
@@ -1114,47 +1146,44 @@
         <v>78</v>
       </c>
       <c r="F19" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>0.0163</v>
+        <v>0.0337</v>
       </c>
       <c r="H19" s="6" t="n">
         <f aca="false">G19*F19</f>
-        <v>0.0652</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>79</v>
+        <v>0.0337</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>0.0008</v>
+        <v>0.1947</v>
       </c>
       <c r="H20" s="6" t="n">
         <f aca="false">G20*F20</f>
-        <v>0.0128</v>
+        <v>0.9735</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1165,7 +1194,7 @@
         <v>85</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>86</v>
@@ -1174,84 +1203,169 @@
         <v>86</v>
       </c>
       <c r="F21" s="1" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>0.0018</v>
+        <v>0.0163</v>
       </c>
       <c r="H21" s="6" t="n">
         <f aca="false">G21*F21</f>
-        <v>0.0396</v>
+        <v>0.0652</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F22" s="1" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G22" s="1" t="n">
-        <v>0.1684</v>
+        <v>0.0008</v>
       </c>
       <c r="H22" s="6" t="n">
         <f aca="false">G22*F22</f>
-        <v>0.1684</v>
+        <v>0.0128</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>0.0018</v>
+      </c>
+      <c r="H23" s="6" t="n">
+        <f aca="false">G23*F23</f>
+        <v>0.0396</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F23" s="8" t="n">
+      <c r="B24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>0.1862</v>
+      </c>
+      <c r="H24" s="6" t="n">
+        <f aca="false">G24*F24</f>
+        <v>0.1862</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>0.2691</v>
+      </c>
+      <c r="H25" s="6" t="n">
+        <f aca="false">G25*F25</f>
+        <v>0.2691</v>
+      </c>
+    </row>
+    <row r="26" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="9" t="n">
-        <f aca="false">G23*F23</f>
+      <c r="H26" s="9" t="n">
+        <f aca="false">G26*F26</f>
         <v>0</v>
       </c>
-      <c r="I23" s="10"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G25" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H25" s="1" t="n">
-        <f aca="false">SUM(H2:H24)</f>
-        <v>7.4139</v>
+      <c r="I26" s="10"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <f aca="false">SUM(H2:H27)</f>
+        <v>7.6315</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H14 H16:H23">
+  <conditionalFormatting sqref="H25:H26 H18:H23 H2:H16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1263,7 +1377,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G23">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1275,8 +1389,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+  <conditionalFormatting sqref="H17">
     <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFE8F2A1"/>
+        <color rgb="FFFFD8CE"/>
+        <color rgb="FFFF6D6D"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24:H25">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>